<commit_message>
group updated due to two dimensional declaration issue
</commit_message>
<xml_diff>
--- a/tutorials/spa-technical-events-automation-user-task/OrderDetailsAssistant.xlsx
+++ b/tutorials/spa-technical-events-automation-user-task/OrderDetailsAssistant.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sap-my.sharepoint.com/personal/celine_audin_sap_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\sap-build-process-automation-Contribution\tutorials\spa-technical-events-automation-user-task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{1B7B94EB-6B6B-416F-A4B0-58EF369CDBC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0FAE718-D4FD-43E6-98CA-9699C856E2E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{41A397A5-BAF1-4144-A974-15564036F59F}"/>
+    <workbookView xWindow="2805" yWindow="-21720" windowWidth="51840" windowHeight="21120" xr2:uid="{41A397A5-BAF1-4144-A974-15564036F59F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -85,7 +85,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,13 +96,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -205,15 +198,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -222,54 +211,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -298,9 +286,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1844040</xdr:colOff>
+      <xdr:colOff>1849482</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>175724</xdr:rowOff>
+      <xdr:rowOff>170282</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -636,214 +624,221 @@
   <dimension ref="B3:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:D12"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.05078125" customWidth="1"/>
-    <col min="3" max="3" width="20.578125" customWidth="1"/>
-    <col min="4" max="4" width="22.89453125" customWidth="1"/>
-    <col min="5" max="5" width="40.578125" customWidth="1"/>
+    <col min="1" max="1" width="13.53515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35" customWidth="1"/>
+    <col min="3" max="3" width="20.53515625" customWidth="1"/>
+    <col min="4" max="4" width="22.84375" customWidth="1"/>
+    <col min="5" max="5" width="40.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C3" s="13" t="s">
+    <row r="3" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C4" s="13"/>
-      <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D3" s="19"/>
+    </row>
+    <row r="4" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C4" s="18"/>
+      <c r="D4" s="19"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C6" s="25" t="s">
+      <c r="D5" s="11"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C7" s="25" t="s">
+      <c r="D6" s="11"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="14" t="s">
+      <c r="D7" s="11"/>
+    </row>
+    <row r="10" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-    </row>
-    <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="12"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="17" t="s">
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+    </row>
+    <row r="11" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="15"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="12"/>
-    </row>
-    <row r="13" spans="2:5" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="17" t="s">
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B13" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="12"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="17" t="s">
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B14" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="12"/>
-    </row>
-    <row r="15" spans="2:5" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="17" t="s">
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B15" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="12"/>
-    </row>
-    <row r="16" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B16" s="19" t="s">
+      <c r="C15" s="21"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="11"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B19" s="4"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-    </row>
-    <row r="20" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B20" s="14" t="s">
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="7"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B19" s="2"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B21" s="14"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="5"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B22" s="2" t="s">
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="15"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B22" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="22"/>
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B23" s="8"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="10"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B24" s="3"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B25" s="3"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="5"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B26" s="3"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B27" s="3"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B28" s="2" t="s">
+      <c r="D22" s="17"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B23" s="13"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B24" s="11"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B25" s="11"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B26" s="11"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B27" s="11"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B28" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D28" s="22"/>
-      <c r="E28" s="12"/>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B29" s="3"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="11"/>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B30" s="3"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="11"/>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B31" s="3"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="11"/>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B32" s="3"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="11"/>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B33" s="3"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="11"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B29" s="11"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="7"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B30" s="11"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="7"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B31" s="11"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="7"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B32" s="11"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="7"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B33" s="11"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C3:D4"/>
+    <mergeCell ref="B10:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="B20:D21"/>
     <mergeCell ref="C28:D28"/>
@@ -857,13 +852,6 @@
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C3:D4"/>
-    <mergeCell ref="B10:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C15:D15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>